<commit_message>
feat: ajuste en importar detalles de salida  y entrega
</commit_message>
<xml_diff>
--- a/src/assets/ejemplos/documentoDetalle/500.xlsx
+++ b/src/assets/ejemplos/documentoDetalle/500.xlsx
@@ -41,7 +41,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -62,14 +62,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,12 +106,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -312,36 +300,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.11"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -358,7 +339,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>